<commit_message>
valor e registro 0507
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/crmpro/TestData.xlsx
+++ b/src/main/resources/testdata/crmpro/TestData.xlsx
@@ -108,15 +108,6 @@
     <t>Inmetrics</t>
   </si>
   <si>
-    <t>Failed - Incorrect Not Found in file</t>
-  </si>
-  <si>
-    <t>MerchantNotFound</t>
-  </si>
-  <si>
-    <t>Failed - Incorrect Not Found in file - Not found WebSite</t>
-  </si>
-  <si>
     <t>Merchant Name</t>
   </si>
   <si>
@@ -126,14 +117,23 @@
     <t xml:space="preserve">http://www.inmetrics.com.br </t>
   </si>
   <si>
-    <t xml:space="preserve">http://www.notfound.com.br </t>
+    <t>PGW00DD5</t>
+  </si>
+  <si>
+    <t>Failed - Incorrect "Amount"</t>
+  </si>
+  <si>
+    <t>GPR01263</t>
+  </si>
+  <si>
+    <t>Failed - Incorrect "CaptureMethod Chip requires RecordType 0507 present"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +180,12 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF0000CC"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -242,16 +248,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,7 +572,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,14 +588,14 @@
     <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="57.85546875" customWidth="1"/>
+    <col min="12" max="12" width="61.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -604,7 +610,7 @@
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -614,10 +620,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>13</v>
@@ -627,35 +633,35 @@
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>67700001</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>71</v>
       </c>
-      <c r="D2" s="3">
-        <v>213</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="D2" s="10">
+        <v>20</v>
+      </c>
+      <c r="E2" s="6">
         <v>43140</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>0</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>704746</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>23</v>
+      <c r="K2" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>14</v>
@@ -665,35 +671,35 @@
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>67700001</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>73</v>
       </c>
-      <c r="D3" s="3">
-        <v>135</v>
-      </c>
-      <c r="E3" s="7">
+      <c r="D3" s="10">
+        <v>150</v>
+      </c>
+      <c r="E3" s="6">
         <v>43137</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>0</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>674537</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>23</v>
+      <c r="K3" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>15</v>
@@ -703,35 +709,35 @@
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>67700001</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>72</v>
       </c>
-      <c r="D4" s="3">
-        <v>426</v>
-      </c>
-      <c r="E4" s="7">
+      <c r="D4" s="10">
+        <v>10.02</v>
+      </c>
+      <c r="E4" s="6">
         <v>43374</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>0</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>704537</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>23</v>
+      <c r="K4" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>16</v>
@@ -741,76 +747,76 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="7">
         <v>67700001</v>
       </c>
-      <c r="C5" s="10">
-        <v>74</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="C5" s="7">
+        <v>72</v>
+      </c>
+      <c r="D5" s="12">
         <v>270</v>
       </c>
-      <c r="E5" s="9">
-        <v>43380</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="E5" s="6">
+        <v>43110</v>
+      </c>
+      <c r="F5" s="3">
         <v>0</v>
       </c>
-      <c r="G5" s="11">
-        <v>746537</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>10</v>
+      <c r="G5" s="4">
+        <v>704537</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>23</v>
+      <c r="K5" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="10">
-        <v>67700001</v>
-      </c>
-      <c r="C6" s="10">
-        <v>75</v>
-      </c>
-      <c r="D6" s="3">
-        <v>483</v>
-      </c>
-      <c r="E6" s="9">
-        <v>43380</v>
-      </c>
-      <c r="F6" s="4">
+      <c r="B6" s="7">
+        <v>24041964</v>
+      </c>
+      <c r="C6" s="7">
+        <v>70</v>
+      </c>
+      <c r="D6" s="10">
+        <v>96</v>
+      </c>
+      <c r="E6" s="6">
+        <v>43137</v>
+      </c>
+      <c r="F6" s="3">
         <v>0</v>
       </c>
-      <c r="G6" s="11">
-        <v>746537</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="10" t="s">
+      <c r="G6" s="4">
+        <v>611867</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>